<commit_message>
Reports: LOI adds row when selected DDV entries > 8
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_13.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -107,10 +107,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="[$-3409]mmmm\ dd\,\ yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-3409]mmmm\ dd\,\ yyyy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -211,11 +211,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -250,7 +250,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -272,13 +272,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -303,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,7 +324,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -336,34 +361,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -673,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:AH197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -703,12 +706,12 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="53">
         <f ca="1">NOW()</f>
-        <v>43670.449224074073</v>
+        <v>43704.645812268522</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -789,17 +792,17 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
@@ -848,13 +851,13 @@
       <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -919,6 +922,7 @@
       <c r="B17" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -933,16 +937,16 @@
     <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -971,12 +975,12 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="48">
+      <c r="G20" s="57">
         <f ca="1">A5</f>
-        <v>43670.449224074073</v>
+        <v>43704.645812268522</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
       <c r="J20" s="16" t="s">
         <v>11</v>
       </c>
@@ -987,16 +991,16 @@
         <v>12</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
       <c r="M21" s="17"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -1007,16 +1011,16 @@
       <c r="T21" s="18"/>
     </row>
     <row r="22" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="53">
+      <c r="D22" s="51">
         <f>J30</f>
         <v>0</v>
       </c>
-      <c r="E22" s="53"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="18" t="s">
         <v>14</v>
       </c>
@@ -1060,93 +1064,93 @@
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:34" s="21" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54" t="s">
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54" t="s">
+      <c r="F25" s="52"/>
+      <c r="G25" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54" t="s">
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
       <c r="M25" s="22"/>
       <c r="O25" s="22"/>
     </row>
     <row r="26" spans="1:34" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
       <c r="M26" s="22"/>
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:34" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
       <c r="M27" s="22"/>
       <c r="O27" s="22"/>
     </row>
     <row r="28" spans="1:34" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
       <c r="M28" s="22"/>
       <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:34" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
       <c r="M29" s="22"/>
       <c r="O29" s="22"/>
     </row>
-    <row r="30" spans="1:34" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
@@ -1178,7 +1182,7 @@
       <c r="AC30" s="4"/>
       <c r="AD30" s="4"/>
     </row>
-    <row r="31" spans="1:34" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -1210,7 +1214,7 @@
       <c r="AC31" s="4"/>
       <c r="AD31" s="4"/>
     </row>
-    <row r="32" spans="1:34" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
@@ -1226,7 +1230,7 @@
       <c r="M32" s="28"/>
       <c r="O32" s="29"/>
     </row>
-    <row r="33" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
@@ -1242,7 +1246,7 @@
       <c r="M33" s="28"/>
       <c r="O33" s="29"/>
     </row>
-    <row r="34" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -1258,7 +1262,7 @@
       <c r="M34" s="30"/>
       <c r="O34" s="29"/>
     </row>
-    <row r="35" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42"/>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -1274,7 +1278,7 @@
       <c r="M35" s="30"/>
       <c r="O35" s="29"/>
     </row>
-    <row r="36" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
@@ -1290,7 +1294,7 @@
       <c r="M36" s="28"/>
       <c r="O36" s="29"/>
     </row>
-    <row r="37" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1306,7 +1310,7 @@
       <c r="M37" s="28"/>
       <c r="O37" s="29"/>
     </row>
-    <row r="38" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
@@ -1322,7 +1326,7 @@
       <c r="M38" s="28"/>
       <c r="O38" s="29"/>
     </row>
-    <row r="39" spans="1:20" s="57" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" s="44" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1344,7 +1348,7 @@
       <c r="S39" s="31"/>
       <c r="T39" s="31"/>
     </row>
-    <row r="40" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1359,7 +1363,7 @@
       <c r="L40" s="38"/>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="1:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
@@ -1374,7 +1378,7 @@
       <c r="L41" s="38"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -1389,7 +1393,7 @@
       <c r="L42" s="38"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1404,7 +1408,7 @@
       <c r="L43" s="38"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" s="35"/>
       <c r="C44" s="35"/>
@@ -1419,7 +1423,7 @@
       <c r="L44" s="40"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
@@ -1434,7 +1438,7 @@
       <c r="L45" s="40"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1449,7 +1453,7 @@
       <c r="L46" s="38"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:20" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -1464,7 +1468,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:20" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
       <c r="C48" s="34"/>
@@ -1479,7 +1483,7 @@
       <c r="L48" s="41"/>
       <c r="M48" s="4"/>
     </row>
-    <row r="49" spans="1:13" s="57" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="44" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
       <c r="C49" s="34"/>
@@ -1493,7 +1497,7 @@
       <c r="K49" s="41"/>
       <c r="L49" s="41"/>
     </row>
-    <row r="50" spans="1:13" s="57" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="44" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
       <c r="C50" s="34"/>
@@ -1507,7 +1511,7 @@
       <c r="K50" s="41"/>
       <c r="L50" s="41"/>
     </row>
-    <row r="51" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1522,7 +1526,7 @@
       <c r="L51" s="38"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1537,7 +1541,7 @@
       <c r="L52" s="38"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1552,7 +1556,7 @@
       <c r="L53" s="38"/>
       <c r="M53" s="4"/>
     </row>
-    <row r="54" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1567,7 +1571,7 @@
       <c r="L54" s="38"/>
       <c r="M54" s="4"/>
     </row>
-    <row r="55" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1582,7 +1586,7 @@
       <c r="L55" s="38"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1597,7 +1601,7 @@
       <c r="L56" s="38"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1612,7 +1616,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1627,7 +1631,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1642,7 +1646,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1657,7 +1661,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1672,7 +1676,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
     </row>
-    <row r="62" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1687,7 +1691,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
     </row>
-    <row r="63" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1702,7 +1706,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1717,7 +1721,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1732,7 +1736,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
     </row>
-    <row r="66" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1747,7 +1751,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1762,7 +1766,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1777,7 +1781,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1792,7 +1796,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1807,7 +1811,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1822,7 +1826,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1837,7 +1841,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
     </row>
-    <row r="73" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1852,7 +1856,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
     </row>
-    <row r="74" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1867,7 +1871,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1882,7 +1886,7 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
     </row>
-    <row r="76" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1897,7 +1901,7 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
     </row>
-    <row r="77" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1912,7 +1916,7 @@
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
     </row>
-    <row r="78" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1927,7 +1931,7 @@
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
     </row>
-    <row r="79" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1942,7 +1946,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
     </row>
-    <row r="80" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1957,7 +1961,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
     </row>
-    <row r="81" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1972,7 +1976,7 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
     </row>
-    <row r="82" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1987,7 +1991,7 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
     </row>
-    <row r="83" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -2002,7 +2006,7 @@
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
     </row>
-    <row r="84" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -2017,7 +2021,7 @@
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
     </row>
-    <row r="85" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2032,7 +2036,7 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
     </row>
-    <row r="86" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2047,7 +2051,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
     </row>
-    <row r="87" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2062,7 +2066,7 @@
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
     </row>
-    <row r="88" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2077,7 +2081,7 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
     </row>
-    <row r="89" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2092,7 +2096,7 @@
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
     </row>
-    <row r="90" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2107,7 +2111,7 @@
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
     </row>
-    <row r="91" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2122,7 +2126,7 @@
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
     </row>
-    <row r="92" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2137,7 +2141,7 @@
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
     </row>
-    <row r="93" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -2152,7 +2156,7 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
     </row>
-    <row r="94" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2167,7 +2171,7 @@
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
     </row>
-    <row r="95" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -2182,7 +2186,7 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
     </row>
-    <row r="96" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -2197,7 +2201,7 @@
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
     </row>
-    <row r="97" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -2212,7 +2216,7 @@
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
     </row>
-    <row r="98" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -2227,7 +2231,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
     </row>
-    <row r="99" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -2242,7 +2246,7 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
     </row>
-    <row r="100" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -2257,7 +2261,7 @@
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
     </row>
-    <row r="101" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -2272,7 +2276,7 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
     </row>
-    <row r="102" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -2287,7 +2291,7 @@
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
     </row>
-    <row r="103" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -2302,7 +2306,7 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
     </row>
-    <row r="104" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -2317,7 +2321,7 @@
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
     </row>
-    <row r="105" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -2332,7 +2336,7 @@
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
     </row>
-    <row r="106" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -2347,7 +2351,7 @@
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
     </row>
-    <row r="107" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -2362,7 +2366,7 @@
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
     </row>
-    <row r="108" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -2377,7 +2381,7 @@
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
     </row>
-    <row r="109" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -2392,7 +2396,7 @@
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
     </row>
-    <row r="110" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -2407,7 +2411,7 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
     </row>
-    <row r="111" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -2422,7 +2426,7 @@
       <c r="L111" s="4"/>
       <c r="M111" s="4"/>
     </row>
-    <row r="112" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -2437,7 +2441,7 @@
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
     </row>
-    <row r="113" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -2452,7 +2456,7 @@
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
     </row>
-    <row r="114" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -2467,7 +2471,7 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
     </row>
-    <row r="115" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -2482,7 +2486,7 @@
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
     </row>
-    <row r="116" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -2497,7 +2501,7 @@
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
     </row>
-    <row r="117" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -2512,7 +2516,7 @@
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
     </row>
-    <row r="118" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -2527,7 +2531,7 @@
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
     </row>
-    <row r="119" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -2542,7 +2546,7 @@
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -2557,7 +2561,7 @@
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
     </row>
-    <row r="121" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -2572,7 +2576,7 @@
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
     </row>
-    <row r="122" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -2587,7 +2591,7 @@
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
     </row>
-    <row r="123" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -2602,7 +2606,7 @@
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
     </row>
-    <row r="124" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -2617,7 +2621,7 @@
       <c r="L124" s="4"/>
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -2632,7 +2636,7 @@
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
     </row>
-    <row r="126" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -2647,7 +2651,7 @@
       <c r="L126" s="4"/>
       <c r="M126" s="4"/>
     </row>
-    <row r="127" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -2662,7 +2666,7 @@
       <c r="L127" s="4"/>
       <c r="M127" s="4"/>
     </row>
-    <row r="128" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -2677,7 +2681,7 @@
       <c r="L128" s="4"/>
       <c r="M128" s="4"/>
     </row>
-    <row r="129" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -2692,7 +2696,7 @@
       <c r="L129" s="4"/>
       <c r="M129" s="4"/>
     </row>
-    <row r="130" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -2707,7 +2711,7 @@
       <c r="L130" s="4"/>
       <c r="M130" s="4"/>
     </row>
-    <row r="131" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -2722,7 +2726,7 @@
       <c r="L131" s="4"/>
       <c r="M131" s="4"/>
     </row>
-    <row r="132" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -2737,7 +2741,7 @@
       <c r="L132" s="4"/>
       <c r="M132" s="4"/>
     </row>
-    <row r="133" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -2752,7 +2756,7 @@
       <c r="L133" s="4"/>
       <c r="M133" s="4"/>
     </row>
-    <row r="134" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -2767,7 +2771,7 @@
       <c r="L134" s="4"/>
       <c r="M134" s="4"/>
     </row>
-    <row r="135" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -2782,7 +2786,7 @@
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
     </row>
-    <row r="136" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -2797,7 +2801,7 @@
       <c r="L136" s="4"/>
       <c r="M136" s="4"/>
     </row>
-    <row r="137" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -2812,7 +2816,7 @@
       <c r="L137" s="4"/>
       <c r="M137" s="4"/>
     </row>
-    <row r="138" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -2827,7 +2831,7 @@
       <c r="L138" s="4"/>
       <c r="M138" s="4"/>
     </row>
-    <row r="139" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -2842,7 +2846,7 @@
       <c r="L139" s="4"/>
       <c r="M139" s="4"/>
     </row>
-    <row r="140" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -2857,7 +2861,7 @@
       <c r="L140" s="4"/>
       <c r="M140" s="4"/>
     </row>
-    <row r="141" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -2872,7 +2876,7 @@
       <c r="L141" s="4"/>
       <c r="M141" s="4"/>
     </row>
-    <row r="142" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -2887,7 +2891,7 @@
       <c r="L142" s="4"/>
       <c r="M142" s="4"/>
     </row>
-    <row r="143" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -2902,7 +2906,7 @@
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
     </row>
-    <row r="144" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -2917,7 +2921,7 @@
       <c r="L144" s="4"/>
       <c r="M144" s="4"/>
     </row>
-    <row r="145" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -2932,7 +2936,7 @@
       <c r="L145" s="4"/>
       <c r="M145" s="4"/>
     </row>
-    <row r="146" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -2947,7 +2951,7 @@
       <c r="L146" s="4"/>
       <c r="M146" s="4"/>
     </row>
-    <row r="147" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -2962,7 +2966,7 @@
       <c r="L147" s="4"/>
       <c r="M147" s="4"/>
     </row>
-    <row r="148" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -2977,7 +2981,7 @@
       <c r="L148" s="4"/>
       <c r="M148" s="4"/>
     </row>
-    <row r="149" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -2992,7 +2996,7 @@
       <c r="L149" s="4"/>
       <c r="M149" s="4"/>
     </row>
-    <row r="150" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
@@ -3007,7 +3011,7 @@
       <c r="L150" s="4"/>
       <c r="M150" s="4"/>
     </row>
-    <row r="151" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
@@ -3022,7 +3026,7 @@
       <c r="L151" s="4"/>
       <c r="M151" s="4"/>
     </row>
-    <row r="152" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
@@ -3037,7 +3041,7 @@
       <c r="L152" s="4"/>
       <c r="M152" s="4"/>
     </row>
-    <row r="153" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
@@ -3052,7 +3056,7 @@
       <c r="L153" s="4"/>
       <c r="M153" s="4"/>
     </row>
-    <row r="154" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
@@ -3067,7 +3071,7 @@
       <c r="L154" s="4"/>
       <c r="M154" s="4"/>
     </row>
-    <row r="155" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
@@ -3082,7 +3086,7 @@
       <c r="L155" s="4"/>
       <c r="M155" s="4"/>
     </row>
-    <row r="156" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
@@ -3097,7 +3101,7 @@
       <c r="L156" s="4"/>
       <c r="M156" s="4"/>
     </row>
-    <row r="157" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
@@ -3112,7 +3116,7 @@
       <c r="L157" s="4"/>
       <c r="M157" s="4"/>
     </row>
-    <row r="158" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -3127,7 +3131,7 @@
       <c r="L158" s="4"/>
       <c r="M158" s="4"/>
     </row>
-    <row r="159" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -3142,7 +3146,7 @@
       <c r="L159" s="4"/>
       <c r="M159" s="4"/>
     </row>
-    <row r="160" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
@@ -3157,7 +3161,7 @@
       <c r="L160" s="4"/>
       <c r="M160" s="4"/>
     </row>
-    <row r="161" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -3172,7 +3176,7 @@
       <c r="L161" s="4"/>
       <c r="M161" s="4"/>
     </row>
-    <row r="162" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
@@ -3187,7 +3191,7 @@
       <c r="L162" s="4"/>
       <c r="M162" s="4"/>
     </row>
-    <row r="163" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -3202,7 +3206,7 @@
       <c r="L163" s="4"/>
       <c r="M163" s="4"/>
     </row>
-    <row r="164" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -3217,7 +3221,7 @@
       <c r="L164" s="4"/>
       <c r="M164" s="4"/>
     </row>
-    <row r="165" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
@@ -3232,7 +3236,7 @@
       <c r="L165" s="4"/>
       <c r="M165" s="4"/>
     </row>
-    <row r="166" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -3247,7 +3251,7 @@
       <c r="L166" s="4"/>
       <c r="M166" s="4"/>
     </row>
-    <row r="167" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -3262,7 +3266,7 @@
       <c r="L167" s="4"/>
       <c r="M167" s="4"/>
     </row>
-    <row r="168" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -3277,7 +3281,7 @@
       <c r="L168" s="4"/>
       <c r="M168" s="4"/>
     </row>
-    <row r="169" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -3292,7 +3296,7 @@
       <c r="L169" s="4"/>
       <c r="M169" s="4"/>
     </row>
-    <row r="170" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
@@ -3307,7 +3311,7 @@
       <c r="L170" s="4"/>
       <c r="M170" s="4"/>
     </row>
-    <row r="171" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
@@ -3322,7 +3326,7 @@
       <c r="L171" s="4"/>
       <c r="M171" s="4"/>
     </row>
-    <row r="172" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -3337,7 +3341,7 @@
       <c r="L172" s="4"/>
       <c r="M172" s="4"/>
     </row>
-    <row r="173" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -3352,7 +3356,7 @@
       <c r="L173" s="4"/>
       <c r="M173" s="4"/>
     </row>
-    <row r="174" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -3367,7 +3371,7 @@
       <c r="L174" s="4"/>
       <c r="M174" s="4"/>
     </row>
-    <row r="175" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -3382,7 +3386,7 @@
       <c r="L175" s="4"/>
       <c r="M175" s="4"/>
     </row>
-    <row r="176" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -3397,7 +3401,7 @@
       <c r="L176" s="4"/>
       <c r="M176" s="4"/>
     </row>
-    <row r="177" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -3412,7 +3416,7 @@
       <c r="L177" s="4"/>
       <c r="M177" s="4"/>
     </row>
-    <row r="178" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -3427,7 +3431,7 @@
       <c r="L178" s="4"/>
       <c r="M178" s="4"/>
     </row>
-    <row r="179" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
@@ -3442,7 +3446,7 @@
       <c r="L179" s="4"/>
       <c r="M179" s="4"/>
     </row>
-    <row r="180" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -3457,7 +3461,7 @@
       <c r="L180" s="4"/>
       <c r="M180" s="4"/>
     </row>
-    <row r="181" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
@@ -3472,7 +3476,7 @@
       <c r="L181" s="4"/>
       <c r="M181" s="4"/>
     </row>
-    <row r="182" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
@@ -3487,7 +3491,7 @@
       <c r="L182" s="4"/>
       <c r="M182" s="4"/>
     </row>
-    <row r="183" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
@@ -3502,7 +3506,7 @@
       <c r="L183" s="4"/>
       <c r="M183" s="4"/>
     </row>
-    <row r="184" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
@@ -3517,7 +3521,7 @@
       <c r="L184" s="4"/>
       <c r="M184" s="4"/>
     </row>
-    <row r="185" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
@@ -3532,7 +3536,7 @@
       <c r="L185" s="4"/>
       <c r="M185" s="4"/>
     </row>
-    <row r="186" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
@@ -3547,7 +3551,7 @@
       <c r="L186" s="4"/>
       <c r="M186" s="4"/>
     </row>
-    <row r="187" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -3562,7 +3566,7 @@
       <c r="L187" s="4"/>
       <c r="M187" s="4"/>
     </row>
-    <row r="188" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
@@ -3577,7 +3581,7 @@
       <c r="L188" s="4"/>
       <c r="M188" s="4"/>
     </row>
-    <row r="189" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -3592,7 +3596,7 @@
       <c r="L189" s="4"/>
       <c r="M189" s="4"/>
     </row>
-    <row r="190" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
@@ -3607,7 +3611,7 @@
       <c r="L190" s="4"/>
       <c r="M190" s="4"/>
     </row>
-    <row r="191" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
@@ -3622,7 +3626,7 @@
       <c r="L191" s="4"/>
       <c r="M191" s="4"/>
     </row>
-    <row r="192" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -3637,7 +3641,7 @@
       <c r="L192" s="4"/>
       <c r="M192" s="4"/>
     </row>
-    <row r="193" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -3652,7 +3656,7 @@
       <c r="L193" s="4"/>
       <c r="M193" s="4"/>
     </row>
-    <row r="194" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
@@ -3667,7 +3671,7 @@
       <c r="L194" s="4"/>
       <c r="M194" s="4"/>
     </row>
-    <row r="195" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
@@ -3682,7 +3686,7 @@
       <c r="L195" s="4"/>
       <c r="M195" s="4"/>
     </row>
-    <row r="196" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -3697,7 +3701,7 @@
       <c r="L196" s="4"/>
       <c r="M196" s="4"/>
     </row>
-    <row r="197" spans="1:13" s="57" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
@@ -3714,14 +3718,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="C21:L21"/>
+    <mergeCell ref="G20:I20"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:I27"/>
@@ -3736,11 +3737,14 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="J26:L26"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>